<commit_message>
se corrigieron las formulas, varias estaban incongruentes
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/IWM_Historico_estimaciones.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/IWM_Historico_estimaciones.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Documents\IWM\CMMI\Repositorio\Organización\Procesos\Soporte Organizacional\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Documents\IWM\CMMI\GitHUB\Organización\Procesos\Soporte Organizacional\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -308,7 +308,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +471,13 @@
       <b/>
       <sz val="16"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -659,12 +666,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -782,9 +790,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -879,6 +884,19 @@
     <xf numFmtId="0" fontId="11" fillId="10" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -888,23 +906,26 @@
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="12" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
     <cellStyle name="Porcentaje 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1338,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,127 +1379,127 @@
     <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-    </row>
-    <row r="2" spans="2:12" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="59"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-    </row>
-    <row r="3" spans="2:12" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="59"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-    </row>
-    <row r="4" spans="2:12" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-    </row>
-    <row r="5" spans="2:12" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
+    <row r="1" spans="2:12" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+    </row>
+    <row r="2" spans="2:12" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="58"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+    </row>
+    <row r="3" spans="2:12" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="58"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+    </row>
+    <row r="4" spans="2:12" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+    </row>
+    <row r="5" spans="2:12" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
     </row>
     <row r="7" spans="2:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="B7" s="56"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="63" t="s">
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="73">
+      <c r="F7" s="72">
         <f>SUM(F9+F16+F30+F47+F50)</f>
-        <v>276</v>
-      </c>
-      <c r="G7" s="57"/>
-      <c r="H7" s="63" t="s">
+        <v>292</v>
+      </c>
+      <c r="G7" s="56"/>
+      <c r="H7" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="73">
+      <c r="I7" s="72">
         <f>SUM(I9+I16+I30+I47+I50)</f>
-        <v>213</v>
-      </c>
-      <c r="J7" s="57"/>
-      <c r="K7" s="79" t="s">
+        <v>222</v>
+      </c>
+      <c r="J7" s="56"/>
+      <c r="K7" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="L7" s="80"/>
+      <c r="L7" s="79"/>
     </row>
     <row r="8" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="64" t="s">
+      <c r="E8" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="54" t="s">
+      <c r="F8" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="54" t="s">
+      <c r="G8" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="54" t="s">
+      <c r="J8" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="81" t="s">
+      <c r="K8" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="54" t="s">
+      <c r="L8" s="53" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1490,29 +1511,29 @@
         <v>33</v>
       </c>
       <c r="D9" s="28"/>
-      <c r="E9" s="65">
+      <c r="E9" s="64">
         <f>(F9/F7)</f>
-        <v>0.15217391304347827</v>
-      </c>
-      <c r="F9" s="48">
+        <v>0.14383561643835616</v>
+      </c>
+      <c r="F9" s="47">
         <f>SUM(F10:F15)</f>
         <v>42</v>
       </c>
-      <c r="G9" s="53"/>
-      <c r="H9" s="65">
+      <c r="G9" s="52"/>
+      <c r="H9" s="64">
         <f>(I9/I7)</f>
-        <v>0.14084507042253522</v>
-      </c>
-      <c r="I9" s="48">
+        <v>0.13513513513513514</v>
+      </c>
+      <c r="I9" s="47">
         <f>SUM(I10:I15)</f>
         <v>30</v>
       </c>
-      <c r="J9" s="53"/>
-      <c r="K9" s="48">
+      <c r="J9" s="89"/>
+      <c r="K9" s="47">
         <f>SUM(K10:K15)</f>
         <v>36</v>
       </c>
-      <c r="L9" s="53"/>
+      <c r="L9" s="52"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="33"/>
@@ -1520,7 +1541,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="33"/>
-      <c r="E10" s="66"/>
+      <c r="E10" s="65"/>
       <c r="F10" s="32">
         <v>8</v>
       </c>
@@ -1528,7 +1549,7 @@
         <f>(F10/F9)</f>
         <v>0.19047619047619047</v>
       </c>
-      <c r="H10" s="66"/>
+      <c r="H10" s="65"/>
       <c r="I10" s="32">
         <v>5</v>
       </c>
@@ -1541,7 +1562,7 @@
         <v>6.5</v>
       </c>
       <c r="L10" s="35">
-        <f>K10/K9</f>
+        <f>(K10/K9)</f>
         <v>0.18055555555555555</v>
       </c>
     </row>
@@ -1551,7 +1572,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="33"/>
-      <c r="E11" s="66"/>
+      <c r="E11" s="65"/>
       <c r="F11" s="32">
         <v>11</v>
       </c>
@@ -1559,7 +1580,7 @@
         <f>(F11/F9)</f>
         <v>0.26190476190476192</v>
       </c>
-      <c r="H11" s="66"/>
+      <c r="H11" s="65"/>
       <c r="I11" s="32">
         <v>8</v>
       </c>
@@ -1572,7 +1593,7 @@
         <v>9.5</v>
       </c>
       <c r="L11" s="35">
-        <f>K11/K9</f>
+        <f>(K11/K9)</f>
         <v>0.2638888888888889</v>
       </c>
     </row>
@@ -1582,7 +1603,7 @@
         <v>30</v>
       </c>
       <c r="D12" s="33"/>
-      <c r="E12" s="66"/>
+      <c r="E12" s="92"/>
       <c r="F12" s="32">
         <v>1</v>
       </c>
@@ -1590,7 +1611,7 @@
         <f>(F12/F9)</f>
         <v>2.3809523809523808E-2</v>
       </c>
-      <c r="H12" s="66"/>
+      <c r="H12" s="65"/>
       <c r="I12" s="32">
         <v>3</v>
       </c>
@@ -1603,7 +1624,7 @@
         <v>2</v>
       </c>
       <c r="L12" s="35">
-        <f>K12/K9</f>
+        <f>(K12/K9)</f>
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
@@ -1613,7 +1634,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="33"/>
-      <c r="E13" s="66"/>
+      <c r="E13" s="65"/>
       <c r="F13" s="32">
         <v>13</v>
       </c>
@@ -1621,7 +1642,7 @@
         <f>(F13/F9)</f>
         <v>0.30952380952380953</v>
       </c>
-      <c r="H13" s="66"/>
+      <c r="H13" s="65"/>
       <c r="I13" s="32">
         <v>10</v>
       </c>
@@ -1634,7 +1655,7 @@
         <v>11.5</v>
       </c>
       <c r="L13" s="35">
-        <f>K13/K9</f>
+        <f>(K13/K9)</f>
         <v>0.31944444444444442</v>
       </c>
     </row>
@@ -1644,7 +1665,7 @@
         <v>45</v>
       </c>
       <c r="D14" s="33"/>
-      <c r="E14" s="66"/>
+      <c r="E14" s="65"/>
       <c r="F14" s="32">
         <v>1</v>
       </c>
@@ -1652,7 +1673,7 @@
         <f>F14/F9</f>
         <v>2.3809523809523808E-2</v>
       </c>
-      <c r="H14" s="66"/>
+      <c r="H14" s="65"/>
       <c r="I14" s="32">
         <v>1</v>
       </c>
@@ -1675,7 +1696,7 @@
         <v>28</v>
       </c>
       <c r="D15" s="33"/>
-      <c r="E15" s="66"/>
+      <c r="E15" s="65"/>
       <c r="F15" s="32">
         <v>8</v>
       </c>
@@ -1683,7 +1704,7 @@
         <f>(F15/F9)</f>
         <v>0.19047619047619047</v>
       </c>
-      <c r="H15" s="66"/>
+      <c r="H15" s="65"/>
       <c r="I15" s="32">
         <v>3</v>
       </c>
@@ -1696,7 +1717,7 @@
         <v>5.5</v>
       </c>
       <c r="L15" s="35">
-        <f>K15/K9</f>
+        <f>(K15/K9)</f>
         <v>0.15277777777777779</v>
       </c>
     </row>
@@ -1708,83 +1729,83 @@
         <v>27</v>
       </c>
       <c r="D16" s="28"/>
-      <c r="E16" s="65">
+      <c r="E16" s="64">
         <f>(F16/F7)</f>
-        <v>0.14492753623188406</v>
-      </c>
-      <c r="F16" s="48">
+        <v>0.19178082191780821</v>
+      </c>
+      <c r="F16" s="47">
         <f>F17+F25</f>
-        <v>40</v>
-      </c>
-      <c r="G16" s="53"/>
-      <c r="H16" s="65">
+        <v>56</v>
+      </c>
+      <c r="G16" s="89"/>
+      <c r="H16" s="64">
         <f>(I16/I7)</f>
-        <v>0.12676056338028169</v>
-      </c>
-      <c r="I16" s="48">
+        <v>0.16216216216216217</v>
+      </c>
+      <c r="I16" s="47">
         <f>I17+I25</f>
-        <v>27</v>
-      </c>
-      <c r="J16" s="53"/>
+        <v>36</v>
+      </c>
+      <c r="J16" s="89"/>
       <c r="K16" s="27">
         <f>SUM(K17,K25)</f>
-        <v>33.5</v>
-      </c>
-      <c r="L16" s="53"/>
+        <v>46</v>
+      </c>
+      <c r="L16" s="89"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="33"/>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="71">
+      <c r="D17" s="50"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="70">
         <f>SUM(F18:F24)</f>
         <v>23</v>
       </c>
-      <c r="G17" s="50"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="71">
+      <c r="G17" s="49"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="70">
         <f>SUM(I18:I24)</f>
         <v>17</v>
       </c>
-      <c r="J17" s="50"/>
-      <c r="K17" s="74">
+      <c r="J17" s="49"/>
+      <c r="K17" s="73">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="L17" s="50"/>
+      <c r="L17" s="49"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="33"/>
       <c r="C18" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="66"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="65"/>
       <c r="F18" s="32">
         <v>3</v>
       </c>
       <c r="G18" s="35">
         <f>(F18/F16)</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="H18" s="66"/>
+        <v>5.3571428571428568E-2</v>
+      </c>
+      <c r="H18" s="65"/>
       <c r="I18" s="32">
         <v>1</v>
       </c>
       <c r="J18" s="35">
         <f>(I18/I16)</f>
-        <v>3.7037037037037035E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="K18" s="40">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L18" s="35">
-        <f>K18/K16</f>
-        <v>5.9701492537313432E-2</v>
+        <f>(K18/K16)</f>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -1793,29 +1814,29 @@
         <v>25</v>
       </c>
       <c r="D19" s="33"/>
-      <c r="E19" s="66"/>
+      <c r="E19" s="65"/>
       <c r="F19" s="32">
         <v>5</v>
       </c>
       <c r="G19" s="35">
         <f>(F19/F16)</f>
-        <v>0.125</v>
-      </c>
-      <c r="H19" s="66"/>
+        <v>8.9285714285714288E-2</v>
+      </c>
+      <c r="H19" s="65"/>
       <c r="I19" s="32">
         <v>4</v>
       </c>
       <c r="J19" s="35">
         <f>(I19/I16)</f>
-        <v>0.14814814814814814</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K19" s="40">
         <f>AVERAGE(F19,I19)</f>
         <v>4.5</v>
       </c>
       <c r="L19" s="35">
-        <f>K19/K16</f>
-        <v>0.13432835820895522</v>
+        <f>(K19/K16)</f>
+        <v>9.7826086956521743E-2</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -1824,29 +1845,29 @@
         <v>24</v>
       </c>
       <c r="D20" s="33"/>
-      <c r="E20" s="66"/>
+      <c r="E20" s="65"/>
       <c r="F20" s="32">
         <v>8</v>
       </c>
       <c r="G20" s="35">
         <f>(F20/F16)</f>
-        <v>0.2</v>
-      </c>
-      <c r="H20" s="66"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="H20" s="65"/>
       <c r="I20" s="32">
         <v>6</v>
       </c>
       <c r="J20" s="35">
         <f>(I20/I16)</f>
-        <v>0.22222222222222221</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="K20" s="40">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L20" s="35">
-        <f>K20/K16</f>
-        <v>0.20895522388059701</v>
+        <f>(K20/K16)</f>
+        <v>0.15217391304347827</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -1855,21 +1876,21 @@
         <v>47</v>
       </c>
       <c r="D21" s="33"/>
-      <c r="E21" s="66"/>
+      <c r="E21" s="65"/>
       <c r="F21" s="32">
         <v>1</v>
       </c>
       <c r="G21" s="35">
         <f>F21/F16</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H21" s="66"/>
+        <v>1.7857142857142856E-2</v>
+      </c>
+      <c r="H21" s="65"/>
       <c r="I21" s="32">
         <v>1</v>
       </c>
       <c r="J21" s="35">
         <f>I21/I16</f>
-        <v>3.7037037037037035E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="K21" s="40">
         <f t="shared" si="0"/>
@@ -1877,7 +1898,7 @@
       </c>
       <c r="L21" s="35">
         <f>K21/K16</f>
-        <v>2.9850746268656716E-2</v>
+        <v>2.1739130434782608E-2</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -1886,29 +1907,29 @@
         <v>23</v>
       </c>
       <c r="D22" s="33"/>
-      <c r="E22" s="66"/>
+      <c r="E22" s="65"/>
       <c r="F22" s="32">
         <v>1</v>
       </c>
       <c r="G22" s="35">
         <f>(F22/F16)</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H22" s="66"/>
+        <v>1.7857142857142856E-2</v>
+      </c>
+      <c r="H22" s="65"/>
       <c r="I22" s="32">
         <v>1</v>
       </c>
       <c r="J22" s="35">
         <f>(I22/I16)</f>
-        <v>3.7037037037037035E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="K22" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L22" s="35">
-        <f>K22/K16</f>
-        <v>2.9850746268656716E-2</v>
+        <f>(K22/K16)</f>
+        <v>2.1739130434782608E-2</v>
       </c>
     </row>
     <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -1917,85 +1938,85 @@
         <v>48</v>
       </c>
       <c r="D23" s="33"/>
-      <c r="E23" s="66"/>
+      <c r="E23" s="65"/>
       <c r="F23" s="32">
         <v>1</v>
       </c>
       <c r="G23" s="35">
         <f>(F23/F16)</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H23" s="66"/>
+        <v>1.7857142857142856E-2</v>
+      </c>
+      <c r="H23" s="65"/>
       <c r="I23" s="32">
         <v>1</v>
       </c>
       <c r="J23" s="35">
         <f>(I23/I16)</f>
-        <v>3.7037037037037035E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="K23" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L23" s="35">
-        <f>K23/K16</f>
-        <v>2.9850746268656716E-2</v>
+        <f>(K23/K16)</f>
+        <v>2.1739130434782608E-2</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="33"/>
-      <c r="C24" s="85" t="s">
+      <c r="C24" s="81" t="s">
         <v>49</v>
       </c>
       <c r="D24" s="33"/>
-      <c r="E24" s="66"/>
+      <c r="E24" s="65"/>
       <c r="F24" s="32">
         <v>4</v>
       </c>
       <c r="G24" s="35">
         <f>(F24/F16)</f>
-        <v>0.1</v>
-      </c>
-      <c r="H24" s="66"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="H24" s="65"/>
       <c r="I24" s="32">
         <v>3</v>
       </c>
       <c r="J24" s="35">
         <f>(I24/I16)</f>
-        <v>0.1111111111111111</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="K24" s="40">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="L24" s="35">
-        <f>K24/K16</f>
-        <v>0.1044776119402985</v>
+        <f>(K24/K16)</f>
+        <v>7.6086956521739135E-2</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="33"/>
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="51"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="72">
-        <f>F27+F29</f>
-        <v>17</v>
-      </c>
-      <c r="G25" s="50"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="72">
-        <f>I27+I29</f>
-        <v>10</v>
-      </c>
-      <c r="J25" s="50"/>
-      <c r="K25" s="75">
-        <f t="shared" si="0"/>
-        <v>13.5</v>
-      </c>
-      <c r="L25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="90">
+        <f>SUM(F26:F29)</f>
+        <v>33</v>
+      </c>
+      <c r="G25" s="49"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="71">
+        <f>SUM(I26:I29)</f>
+        <v>19</v>
+      </c>
+      <c r="J25" s="49"/>
+      <c r="K25" s="74">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="L25" s="49"/>
     </row>
     <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="33"/>
@@ -2003,29 +2024,29 @@
         <v>50</v>
       </c>
       <c r="D26" s="33"/>
-      <c r="E26" s="66"/>
+      <c r="E26" s="65"/>
       <c r="F26" s="32">
         <v>15</v>
       </c>
       <c r="G26" s="35">
-        <f>(F26/F15)</f>
-        <v>1.875</v>
-      </c>
-      <c r="H26" s="66"/>
+        <f>(F26/F16)</f>
+        <v>0.26785714285714285</v>
+      </c>
+      <c r="H26" s="65"/>
       <c r="I26" s="32">
         <v>8</v>
       </c>
       <c r="J26" s="35">
-        <f>(I26/I15)</f>
-        <v>2.6666666666666665</v>
+        <f>(I26/I16)</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="K26" s="40">
         <f t="shared" ref="K26" si="1">AVERAGE(F26,I26)</f>
         <v>11.5</v>
       </c>
       <c r="L26" s="35">
-        <f>K26/K15</f>
-        <v>2.0909090909090908</v>
+        <f>(K26/K16)</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2034,29 +2055,29 @@
         <v>21</v>
       </c>
       <c r="D27" s="33"/>
-      <c r="E27" s="66"/>
+      <c r="E27" s="65"/>
       <c r="F27" s="32">
         <v>15</v>
       </c>
       <c r="G27" s="35">
         <f>(F27/F16)</f>
-        <v>0.375</v>
-      </c>
-      <c r="H27" s="66"/>
+        <v>0.26785714285714285</v>
+      </c>
+      <c r="H27" s="65"/>
       <c r="I27" s="32">
         <v>8</v>
       </c>
       <c r="J27" s="35">
         <f>(I27/I16)</f>
-        <v>0.29629629629629628</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="K27" s="40">
         <f t="shared" si="0"/>
         <v>11.5</v>
       </c>
       <c r="L27" s="35">
-        <f>K27/K16</f>
-        <v>0.34328358208955223</v>
+        <f>(K27/K16)</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2065,21 +2086,21 @@
         <v>51</v>
       </c>
       <c r="D28" s="33"/>
-      <c r="E28" s="66"/>
+      <c r="E28" s="65"/>
       <c r="F28" s="32">
         <v>1</v>
       </c>
       <c r="G28" s="35">
         <f>F28/F16</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H28" s="66"/>
+        <v>1.7857142857142856E-2</v>
+      </c>
+      <c r="H28" s="65"/>
       <c r="I28" s="32">
         <v>1</v>
       </c>
       <c r="J28" s="35">
         <f>I28/I16</f>
-        <v>3.7037037037037035E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="K28" s="40">
         <f t="shared" si="0"/>
@@ -2087,7 +2108,7 @@
       </c>
       <c r="L28" s="35">
         <f>K28/K16</f>
-        <v>2.9850746268656716E-2</v>
+        <v>2.1739130434782608E-2</v>
       </c>
     </row>
     <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2096,29 +2117,29 @@
         <v>20</v>
       </c>
       <c r="D29" s="33"/>
-      <c r="E29" s="66"/>
+      <c r="E29" s="65"/>
       <c r="F29" s="32">
         <v>2</v>
       </c>
       <c r="G29" s="35">
         <f>(F29/F16)</f>
-        <v>0.05</v>
-      </c>
-      <c r="H29" s="66"/>
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="H29" s="65"/>
       <c r="I29" s="32">
         <v>2</v>
       </c>
       <c r="J29" s="35">
         <f>(I29/I16)</f>
-        <v>7.407407407407407E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="K29" s="40">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L29" s="35">
-        <f>K29/K16</f>
-        <v>5.9701492537313432E-2</v>
+        <f>(K29/K16)</f>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2128,30 +2149,30 @@
       <c r="C30" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="49"/>
-      <c r="E30" s="67">
+      <c r="D30" s="48"/>
+      <c r="E30" s="66">
         <f>SUM(E31+E36+E38+E44)</f>
-        <v>0.50724637681159424</v>
-      </c>
-      <c r="F30" s="48">
+        <v>0.47945205479452058</v>
+      </c>
+      <c r="F30" s="47">
         <f>F31+F36+F38+F44</f>
         <v>140</v>
       </c>
-      <c r="G30" s="47"/>
-      <c r="H30" s="67">
+      <c r="G30" s="93"/>
+      <c r="H30" s="66">
         <f>SUM(H31+H36+H38+H44)</f>
-        <v>0.47887323943661969</v>
-      </c>
-      <c r="I30" s="48">
+        <v>0.45945945945945954</v>
+      </c>
+      <c r="I30" s="47">
         <f>I31+I36+I38+I44</f>
         <v>102</v>
       </c>
-      <c r="J30" s="47"/>
+      <c r="J30" s="93"/>
       <c r="K30" s="27">
         <f t="shared" si="0"/>
         <v>121</v>
       </c>
-      <c r="L30" s="47"/>
+      <c r="L30" s="93"/>
     </row>
     <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="24">
@@ -2161,18 +2182,18 @@
         <v>18</v>
       </c>
       <c r="D31" s="45"/>
-      <c r="E31" s="68">
+      <c r="E31" s="67">
         <f>(F31/F7)</f>
-        <v>5.434782608695652E-2</v>
+        <v>5.1369863013698627E-2</v>
       </c>
       <c r="F31" s="37">
         <f>SUM(F32:F34)</f>
         <v>15</v>
       </c>
       <c r="G31" s="46"/>
-      <c r="H31" s="68">
+      <c r="H31" s="67">
         <f>(I31/I7)</f>
-        <v>3.7558685446009391E-2</v>
+        <v>3.6036036036036036E-2</v>
       </c>
       <c r="I31" s="37">
         <f>SUM(I32:I35)</f>
@@ -2191,7 +2212,7 @@
         <v>52</v>
       </c>
       <c r="D32" s="44"/>
-      <c r="E32" s="66"/>
+      <c r="E32" s="65"/>
       <c r="F32" s="32">
         <v>5</v>
       </c>
@@ -2199,7 +2220,7 @@
         <f>F32/F30</f>
         <v>3.5714285714285712E-2</v>
       </c>
-      <c r="H32" s="66"/>
+      <c r="H32" s="65"/>
       <c r="I32" s="32">
         <v>2</v>
       </c>
@@ -2222,27 +2243,27 @@
         <v>53</v>
       </c>
       <c r="D33" s="44"/>
-      <c r="E33" s="66"/>
-      <c r="F33" s="86">
+      <c r="E33" s="65"/>
+      <c r="F33" s="82">
         <v>5</v>
       </c>
       <c r="G33" s="35">
         <f>F33/F30</f>
         <v>3.5714285714285712E-2</v>
       </c>
-      <c r="H33" s="66"/>
-      <c r="I33" s="86">
+      <c r="H33" s="65"/>
+      <c r="I33" s="82">
         <v>2</v>
       </c>
-      <c r="J33" s="88">
+      <c r="J33" s="84">
         <f>I33/I30</f>
         <v>1.9607843137254902E-2</v>
       </c>
-      <c r="K33" s="87">
+      <c r="K33" s="83">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="L33" s="35">
+      <c r="L33" s="84">
         <f>K33/K30</f>
         <v>2.8925619834710745E-2</v>
       </c>
@@ -2253,27 +2274,27 @@
         <v>54</v>
       </c>
       <c r="D34" s="44"/>
-      <c r="E34" s="66"/>
-      <c r="F34" s="86">
+      <c r="E34" s="65"/>
+      <c r="F34" s="82">
         <v>5</v>
       </c>
       <c r="G34" s="35">
         <f>F34/F30</f>
         <v>3.5714285714285712E-2</v>
       </c>
-      <c r="H34" s="66"/>
-      <c r="I34" s="86">
+      <c r="H34" s="65"/>
+      <c r="I34" s="82">
         <v>2</v>
       </c>
-      <c r="J34" s="88">
+      <c r="J34" s="84">
         <f>I34/I30</f>
         <v>1.9607843137254902E-2</v>
       </c>
-      <c r="K34" s="87">
+      <c r="K34" s="83">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="L34" s="35">
+      <c r="L34" s="84">
         <f>K34/K30</f>
         <v>2.8925619834710745E-2</v>
       </c>
@@ -2284,23 +2305,23 @@
         <v>55</v>
       </c>
       <c r="D35" s="44"/>
-      <c r="E35" s="66"/>
-      <c r="F35" s="86">
+      <c r="E35" s="65"/>
+      <c r="F35" s="82">
         <v>2</v>
       </c>
       <c r="G35" s="35">
         <f>F35/F30</f>
         <v>1.4285714285714285E-2</v>
       </c>
-      <c r="H35" s="66"/>
-      <c r="I35" s="86">
+      <c r="H35" s="65"/>
+      <c r="I35" s="82">
         <v>2</v>
       </c>
       <c r="J35" s="35">
         <f>I35/I30</f>
         <v>1.9607843137254902E-2</v>
       </c>
-      <c r="K35" s="87">
+      <c r="K35" s="83">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2317,18 +2338,18 @@
         <v>17</v>
       </c>
       <c r="D36" s="45"/>
-      <c r="E36" s="68">
+      <c r="E36" s="67">
         <f>(F36/F7)</f>
-        <v>0.34057971014492755</v>
+        <v>0.32191780821917809</v>
       </c>
       <c r="F36" s="37">
         <f>F37</f>
         <v>94</v>
       </c>
       <c r="G36" s="41"/>
-      <c r="H36" s="68">
+      <c r="H36" s="67">
         <f>(I36/I7)</f>
-        <v>0.31455399061032863</v>
+        <v>0.30180180180180183</v>
       </c>
       <c r="I36" s="37">
         <f>I37</f>
@@ -2347,26 +2368,29 @@
         <v>16</v>
       </c>
       <c r="D37" s="44"/>
-      <c r="E37" s="66"/>
+      <c r="E37" s="65"/>
       <c r="F37" s="32">
         <v>94</v>
       </c>
       <c r="G37" s="35">
-        <v>1</v>
-      </c>
-      <c r="H37" s="66"/>
+        <f>F37/F30</f>
+        <v>0.67142857142857137</v>
+      </c>
+      <c r="H37" s="65"/>
       <c r="I37" s="32">
         <v>67</v>
       </c>
       <c r="J37" s="35">
-        <v>1</v>
+        <f>I37/I30</f>
+        <v>0.65686274509803921</v>
       </c>
       <c r="K37" s="40">
         <f t="shared" si="0"/>
         <v>80.5</v>
       </c>
       <c r="L37" s="35">
-        <v>1</v>
+        <f>K37/K30</f>
+        <v>0.66528925619834711</v>
       </c>
     </row>
     <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2377,18 +2401,18 @@
         <v>15</v>
       </c>
       <c r="D38" s="43"/>
-      <c r="E38" s="68">
+      <c r="E38" s="67">
         <f>(F38/F7)</f>
-        <v>4.710144927536232E-2</v>
+        <v>4.4520547945205477E-2</v>
       </c>
       <c r="F38" s="42">
         <f>SUM(F39:F43)</f>
         <v>13</v>
       </c>
       <c r="G38" s="41"/>
-      <c r="H38" s="68">
+      <c r="H38" s="67">
         <f>(I38/I7)</f>
-        <v>6.1032863849765258E-2</v>
+        <v>5.8558558558558557E-2</v>
       </c>
       <c r="I38" s="42">
         <f>SUM(I39:I43)</f>
@@ -2407,26 +2431,29 @@
         <v>14</v>
       </c>
       <c r="D39" s="40"/>
-      <c r="E39" s="66"/>
+      <c r="E39" s="65"/>
       <c r="F39" s="32">
         <v>2</v>
       </c>
       <c r="G39" s="35">
-        <v>0.2</v>
-      </c>
-      <c r="H39" s="66"/>
+        <f>F39/F30</f>
+        <v>1.4285714285714285E-2</v>
+      </c>
+      <c r="H39" s="65"/>
       <c r="I39" s="32">
         <v>2</v>
       </c>
       <c r="J39" s="35">
-        <v>0.2</v>
+        <f>I39/I30</f>
+        <v>1.9607843137254902E-2</v>
       </c>
       <c r="K39" s="40">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L39" s="35">
-        <v>0.2</v>
+        <f>K39/K30</f>
+        <v>1.6528925619834711E-2</v>
       </c>
     </row>
     <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2435,26 +2462,29 @@
         <v>13</v>
       </c>
       <c r="D40" s="40"/>
-      <c r="E40" s="66"/>
+      <c r="E40" s="65"/>
       <c r="F40" s="32">
         <v>4</v>
       </c>
       <c r="G40" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="H40" s="66"/>
+        <f>F40/F30</f>
+        <v>2.8571428571428571E-2</v>
+      </c>
+      <c r="H40" s="65"/>
       <c r="I40" s="32">
         <v>4</v>
       </c>
       <c r="J40" s="35">
-        <v>0.5</v>
+        <f>I40/I30</f>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="K40" s="40">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L40" s="35">
-        <v>0.5</v>
+        <f>K40/K30</f>
+        <v>3.3057851239669422E-2</v>
       </c>
     </row>
     <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2463,26 +2493,29 @@
         <v>12</v>
       </c>
       <c r="D41" s="40"/>
-      <c r="E41" s="66"/>
+      <c r="E41" s="65"/>
       <c r="F41" s="32">
         <v>3</v>
       </c>
       <c r="G41" s="35">
-        <v>0.1</v>
-      </c>
-      <c r="H41" s="66"/>
+        <f>F41/F30</f>
+        <v>2.1428571428571429E-2</v>
+      </c>
+      <c r="H41" s="65"/>
       <c r="I41" s="32">
         <v>3</v>
       </c>
       <c r="J41" s="35">
-        <v>0.1</v>
+        <f>I41/I30</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="K41" s="40">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L41" s="35">
-        <v>0.1</v>
+        <f>K41/K30</f>
+        <v>2.4793388429752067E-2</v>
       </c>
     </row>
     <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2491,26 +2524,29 @@
         <v>41</v>
       </c>
       <c r="D42" s="40"/>
-      <c r="E42" s="66"/>
+      <c r="E42" s="65"/>
       <c r="F42" s="32">
         <v>3</v>
       </c>
       <c r="G42" s="35">
-        <v>0.2</v>
-      </c>
-      <c r="H42" s="66"/>
+        <f>F42/F30</f>
+        <v>2.1428571428571429E-2</v>
+      </c>
+      <c r="H42" s="65"/>
       <c r="I42" s="32">
         <v>3</v>
       </c>
       <c r="J42" s="35">
-        <v>0.2</v>
+        <f>I42/I30</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="K42" s="40">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L42" s="35">
-        <v>0.2</v>
+        <f>K42/K30</f>
+        <v>2.4793388429752067E-2</v>
       </c>
     </row>
     <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2519,26 +2555,29 @@
         <v>40</v>
       </c>
       <c r="D43" s="40"/>
-      <c r="E43" s="66"/>
+      <c r="E43" s="65"/>
       <c r="F43" s="32">
         <v>1</v>
       </c>
       <c r="G43" s="35">
-        <v>0.2</v>
-      </c>
-      <c r="H43" s="66"/>
+        <f>F43/F30</f>
+        <v>7.1428571428571426E-3</v>
+      </c>
+      <c r="H43" s="65"/>
       <c r="I43" s="32">
         <v>1</v>
       </c>
       <c r="J43" s="35">
-        <v>0.2</v>
+        <f>I43/I30</f>
+        <v>9.8039215686274508E-3</v>
       </c>
       <c r="K43" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L43" s="35">
-        <v>0.2</v>
+        <f>K43/K30</f>
+        <v>8.2644628099173556E-3</v>
       </c>
     </row>
     <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2549,18 +2588,18 @@
         <v>11</v>
       </c>
       <c r="D44" s="38"/>
-      <c r="E44" s="68">
+      <c r="E44" s="67">
         <f>(F44/F7)</f>
-        <v>6.5217391304347824E-2</v>
+        <v>6.1643835616438353E-2</v>
       </c>
       <c r="F44" s="37">
         <f>F45+F46</f>
         <v>18</v>
       </c>
       <c r="G44" s="36"/>
-      <c r="H44" s="68">
+      <c r="H44" s="67">
         <f>(I44/I7)</f>
-        <v>6.5727699530516437E-2</v>
+        <v>6.3063063063063057E-2</v>
       </c>
       <c r="I44" s="37">
         <f>I45+I46</f>
@@ -2579,26 +2618,29 @@
         <v>10</v>
       </c>
       <c r="D45" s="33"/>
-      <c r="E45" s="66"/>
+      <c r="E45" s="65"/>
       <c r="F45" s="32">
         <v>9</v>
       </c>
       <c r="G45" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="H45" s="66"/>
+        <f>F45/F30</f>
+        <v>6.4285714285714279E-2</v>
+      </c>
+      <c r="H45" s="65"/>
       <c r="I45" s="32">
         <v>7</v>
       </c>
       <c r="J45" s="35">
-        <v>0.5</v>
+        <f>I45/I30</f>
+        <v>6.8627450980392163E-2</v>
       </c>
       <c r="K45" s="40">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L45" s="35">
-        <v>0.5</v>
+        <f>K45/K30</f>
+        <v>6.6115702479338845E-2</v>
       </c>
     </row>
     <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2607,26 +2649,29 @@
         <v>9</v>
       </c>
       <c r="D46" s="33"/>
-      <c r="E46" s="66"/>
+      <c r="E46" s="65"/>
       <c r="F46" s="32">
         <v>9</v>
       </c>
       <c r="G46" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="H46" s="66"/>
+        <f>F46/F30</f>
+        <v>6.4285714285714279E-2</v>
+      </c>
+      <c r="H46" s="65"/>
       <c r="I46" s="32">
         <v>7</v>
       </c>
       <c r="J46" s="35">
-        <v>0.5</v>
+        <f>I46/I30</f>
+        <v>6.8627450980392163E-2</v>
       </c>
       <c r="K46" s="40">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L46" s="35">
-        <v>0.5</v>
+        <f>K46/K30</f>
+        <v>6.6115702479338845E-2</v>
       </c>
     </row>
     <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2637,18 +2682,18 @@
         <v>8</v>
       </c>
       <c r="D47" s="28"/>
-      <c r="E47" s="65">
+      <c r="E47" s="64">
         <f>(F47/F7)</f>
-        <v>2.8985507246376812E-2</v>
+        <v>2.7397260273972601E-2</v>
       </c>
       <c r="F47" s="27">
         <f>SUM(F48:F49)</f>
         <v>8</v>
       </c>
       <c r="G47" s="26"/>
-      <c r="H47" s="65">
+      <c r="H47" s="64">
         <f>(I47/I7)</f>
-        <v>3.7558685446009391E-2</v>
+        <v>3.6036036036036036E-2</v>
       </c>
       <c r="I47" s="27">
         <f>SUM(I48:I49)</f>
@@ -2669,7 +2714,7 @@
         <v>56</v>
       </c>
       <c r="D48" s="33"/>
-      <c r="E48" s="66"/>
+      <c r="E48" s="65"/>
       <c r="F48" s="32">
         <v>4</v>
       </c>
@@ -2677,7 +2722,7 @@
         <f>F48/F47</f>
         <v>0.5</v>
       </c>
-      <c r="H48" s="66"/>
+      <c r="H48" s="65"/>
       <c r="I48" s="32">
         <v>4</v>
       </c>
@@ -2700,16 +2745,16 @@
         <v>57</v>
       </c>
       <c r="D49" s="33"/>
-      <c r="E49" s="89"/>
-      <c r="F49" s="86">
+      <c r="E49" s="85"/>
+      <c r="F49" s="82">
         <v>4</v>
       </c>
       <c r="G49" s="31">
         <f>F49/F47</f>
         <v>0.5</v>
       </c>
-      <c r="H49" s="89"/>
-      <c r="I49" s="86">
+      <c r="H49" s="85"/>
+      <c r="I49" s="82">
         <v>4</v>
       </c>
       <c r="J49" s="31">
@@ -2733,18 +2778,18 @@
         <v>7</v>
       </c>
       <c r="D50" s="28"/>
-      <c r="E50" s="69">
+      <c r="E50" s="68">
         <f>(F50/F7)</f>
-        <v>0.16666666666666666</v>
+        <v>0.15753424657534246</v>
       </c>
       <c r="F50" s="27">
         <f>SUM(F51:F54)</f>
         <v>46</v>
       </c>
       <c r="G50" s="26"/>
-      <c r="H50" s="69">
+      <c r="H50" s="68">
         <f>(I50/I7)</f>
-        <v>0.215962441314554</v>
+        <v>0.2072072072072072</v>
       </c>
       <c r="I50" s="27">
         <f>SUM(I51:I54)</f>
@@ -2763,7 +2808,7 @@
         <v>6</v>
       </c>
       <c r="D51" s="19"/>
-      <c r="E51" s="66"/>
+      <c r="E51" s="65"/>
       <c r="F51" s="22">
         <v>12</v>
       </c>
@@ -2771,7 +2816,7 @@
         <f>(F51/F50)</f>
         <v>0.2608695652173913</v>
       </c>
-      <c r="H51" s="66"/>
+      <c r="H51" s="65"/>
       <c r="I51" s="22">
         <v>12</v>
       </c>
@@ -2779,7 +2824,7 @@
         <f>(I51/I50)</f>
         <v>0.2608695652173913</v>
       </c>
-      <c r="K51" s="76">
+      <c r="K51" s="75">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2796,7 +2841,7 @@
         <v>5</v>
       </c>
       <c r="D52" s="19"/>
-      <c r="E52" s="66"/>
+      <c r="E52" s="65"/>
       <c r="F52" s="22">
         <v>24</v>
       </c>
@@ -2804,7 +2849,7 @@
         <f>(F52/F50)</f>
         <v>0.52173913043478259</v>
       </c>
-      <c r="H52" s="66"/>
+      <c r="H52" s="65"/>
       <c r="I52" s="22">
         <v>24</v>
       </c>
@@ -2812,7 +2857,7 @@
         <f>(I52/I50)</f>
         <v>0.52173913043478259</v>
       </c>
-      <c r="K52" s="76">
+      <c r="K52" s="75">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -2829,7 +2874,7 @@
         <v>4</v>
       </c>
       <c r="D53" s="19"/>
-      <c r="E53" s="66"/>
+      <c r="E53" s="65"/>
       <c r="F53" s="22">
         <v>4</v>
       </c>
@@ -2837,7 +2882,7 @@
         <f>(F53/F50)</f>
         <v>8.6956521739130432E-2</v>
       </c>
-      <c r="H53" s="66"/>
+      <c r="H53" s="65"/>
       <c r="I53" s="22">
         <v>4</v>
       </c>
@@ -2845,7 +2890,7 @@
         <f>(I53/I50)</f>
         <v>8.6956521739130432E-2</v>
       </c>
-      <c r="K53" s="76">
+      <c r="K53" s="75">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -2862,7 +2907,7 @@
         <v>3</v>
       </c>
       <c r="D54" s="19"/>
-      <c r="E54" s="66"/>
+      <c r="E54" s="65"/>
       <c r="F54" s="18">
         <v>6</v>
       </c>
@@ -2870,7 +2915,7 @@
         <f>(F54/F50)</f>
         <v>0.13043478260869565</v>
       </c>
-      <c r="H54" s="66"/>
+      <c r="H54" s="65"/>
       <c r="I54" s="18">
         <v>6</v>
       </c>
@@ -2878,7 +2923,7 @@
         <f>(I54/I50)</f>
         <v>0.13043478260869565</v>
       </c>
-      <c r="K54" s="77">
+      <c r="K54" s="76">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -2896,19 +2941,19 @@
         <v>2</v>
       </c>
       <c r="D55" s="13"/>
-      <c r="E55" s="70"/>
+      <c r="E55" s="69"/>
       <c r="F55" s="12" t="s">
         <v>0</v>
       </c>
       <c r="G55" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="H55" s="70"/>
+      <c r="H55" s="69"/>
       <c r="I55" s="12"/>
       <c r="J55" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="K55" s="78"/>
+      <c r="K55" s="77"/>
       <c r="L55" s="11" t="s">
         <v>0</v>
       </c>
@@ -2951,8 +2996,8 @@
       <c r="D63" s="5"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C64" s="82"/>
-      <c r="D64" s="82"/>
+      <c r="C64" s="86"/>
+      <c r="D64" s="86"/>
     </row>
     <row r="65" spans="3:3" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>